<commit_message>
new version of assets; logging added; add 'teamNameAlreadyExists' error handling;
</commit_message>
<xml_diff>
--- a/assets/TEAMS_SETUP_5.xlsx
+++ b/assets/TEAMS_SETUP_5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr backupFile="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Игорь\WebstormProjects\synchroreg\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447F0DFB-93BA-45BC-9945-4251FF417C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7DA28A-995A-43D4-BB81-3EFF6157CC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -291,7 +291,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>судья</t>
   </si>
@@ -345,12 +345,6 @@
   </si>
   <si>
     <t>Регион</t>
-  </si>
-  <si>
-    <t>сопровождающий</t>
-  </si>
-  <si>
-    <t>врач</t>
   </si>
   <si>
     <t>Страна</t>
@@ -1506,10 +1500,10 @@
   <dimension ref="A1:AK75"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="AH5" sqref="AG5:AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1562,13 +1556,13 @@
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
       <c r="J1" s="67" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K1" s="44"/>
       <c r="L1" s="44"/>
       <c r="M1" s="65"/>
       <c r="N1" s="67" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O1" s="65"/>
       <c r="P1" s="65"/>
@@ -1576,13 +1570,13 @@
       <c r="R1" s="65"/>
       <c r="S1" s="66"/>
       <c r="T1" s="67" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="U1" s="68"/>
       <c r="V1" s="68"/>
       <c r="W1" s="69"/>
       <c r="X1" s="88" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Z1" s="28" t="s">
         <v>11</v>
@@ -1595,7 +1589,7 @@
     <row r="2" spans="1:37" s="23" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="B2" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="38"/>
       <c r="D2" s="20"/>
@@ -1696,7 +1690,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>3</v>
@@ -1708,50 +1702,50 @@
         <v>16</v>
       </c>
       <c r="H3" s="42" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="75" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K3" s="87" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="87" t="s">
+      <c r="M3" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="79" t="s">
-        <v>40</v>
-      </c>
       <c r="N3" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="S3" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="46" t="s">
+      <c r="T3" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="V3" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="S3" s="45" t="s">
+      <c r="W3" s="55" t="s">
         <v>28</v>
-      </c>
-      <c r="T3" s="53" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="V3" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="W3" s="55" t="s">
-        <v>30</v>
       </c>
       <c r="Y3" s="15"/>
       <c r="Z3" s="15" t="s">
@@ -1761,7 +1755,7 @@
         <v>17</v>
       </c>
       <c r="AB3" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AC3" s="15" t="s">
         <v>12</v>
@@ -1816,9 +1810,6 @@
         <f t="shared" ref="AD4:AD46" si="1">COUNTIF($AH:$AH,$Z4)</f>
         <v>0</v>
       </c>
-      <c r="AF4" s="7">
-        <v>1</v>
-      </c>
       <c r="AK4" s="34" t="s">
         <v>0</v>
       </c>
@@ -1846,9 +1837,6 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AF5" s="7">
-        <v>2</v>
-      </c>
       <c r="AK5" s="34" t="s">
         <v>1</v>
       </c>
@@ -1876,9 +1864,6 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AF6" s="7">
-        <v>3</v>
-      </c>
       <c r="AK6" s="34" t="s">
         <v>4</v>
       </c>
@@ -1906,9 +1891,6 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AK7" s="34" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="8" spans="1:37" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="35"/>
@@ -1932,9 +1914,6 @@
       <c r="AD8" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="AK8" s="34" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:37" ht="15" x14ac:dyDescent="0.25">

</xml_diff>